<commit_message>
results - two patterns and two lead ecg order fix
</commit_message>
<xml_diff>
--- a/paper/ProximityForestUCRResultsCombined.xlsx
+++ b/paper/ProximityForestUCRResultsCombined.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shifaz/git/github/ProximityForest/paper/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\ProximityForest\paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16500" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="r=5" sheetId="1" r:id="rId1"/>
@@ -346,7 +346,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -387,6 +387,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -657,16 +660,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:G1048576"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75:G76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -707,7 +710,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -751,7 +754,7 @@
         <v>14477.8789919677</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -795,7 +798,7 @@
         <v>5799.9433176592302</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -839,7 +842,7 @@
         <v>6485.3903472278998</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -883,7 +886,7 @@
         <v>1049.60349369153</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -927,7 +930,7 @@
         <v>598.93792821901195</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -971,7 +974,7 @@
         <v>3450.6730708631399</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1015,7 +1018,7 @@
         <v>2381.05945797698</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1059,7 +1062,7 @@
         <v>22597.6484765319</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1103,7 +1106,7 @@
         <v>1905920.7602634199</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1147,7 +1150,7 @@
         <v>217.702889835429</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1191,7 +1194,7 @@
         <v>30055.6815131734</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1235,7 +1238,7 @@
         <v>21455.451344966001</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1279,7 +1282,7 @@
         <v>59117.797884706502</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1323,7 +1326,7 @@
         <v>91468.7946850765</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1367,7 +1370,7 @@
         <v>7665.5888824147596</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1411,7 +1414,7 @@
         <v>204.20824565832601</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1455,7 +1458,7 @@
         <v>274.43374531016002</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1499,7 +1502,7 @@
         <v>141.40422902665301</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>21</v>
       </c>
@@ -1543,7 +1546,7 @@
         <v>50220.175736552199</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
@@ -1587,7 +1590,7 @@
         <v>162.23362777279999</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>19</v>
       </c>
@@ -1631,7 +1634,7 @@
         <v>22855.034088459499</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20</v>
       </c>
@@ -1675,7 +1678,7 @@
         <v>2382.3528901609802</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1719,7 +1722,7 @@
         <v>15670.3513390261</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1763,7 +1766,7 @@
         <v>21635.901293882202</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1807,7 +1810,7 @@
         <v>2495.5105738593702</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1851,7 +1854,7 @@
         <v>27510.0676159041</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1895,7 +1898,7 @@
         <v>176627.24791237499</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1939,7 +1942,7 @@
         <v>10624.9798047188</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1983,7 +1986,7 @@
         <v>730301.91344655398</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -2027,7 +2030,7 @@
         <v>405348.403801721</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -2071,7 +2074,7 @@
         <v>323.662949914563</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -2115,7 +2118,7 @@
         <v>1812.34007552515</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -2159,7 +2162,7 @@
         <v>1820133.2340722899</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -2203,7 +2206,7 @@
         <v>148866.02747104</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
@@ -2247,7 +2250,7 @@
         <v>2141.3612059874699</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -2291,7 +2294,7 @@
         <v>2556134.4460293702</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
@@ -2335,7 +2338,7 @@
         <v>42265.600038045501</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -2379,7 +2382,7 @@
         <v>119.64726978738901</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
@@ -2423,7 +2426,7 @@
         <v>318571.43732017599</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -2467,7 +2470,7 @@
         <v>1976.2383902002</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
@@ -2511,7 +2514,7 @@
         <v>2280.5615925388702</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
@@ -2555,7 +2558,7 @@
         <v>492165.88173796801</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
@@ -2599,7 +2602,7 @@
         <v>2581.8330290310801</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
@@ -2643,7 +2646,7 @@
         <v>3206.2744524528198</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
@@ -2687,7 +2690,7 @@
         <v>1078.9399972398401</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
@@ -2731,7 +2734,7 @@
         <v>430.60587722582102</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
@@ -2775,7 +2778,7 @@
         <v>1234.1716570742601</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
@@ -2819,7 +2822,7 @@
         <v>1086.86364772105</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
@@ -2863,7 +2866,7 @@
         <v>5693685.0748102199</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
@@ -2907,7 +2910,7 @@
         <v>4338385.2769992203</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2951,7 +2954,7 @@
         <v>1466.56093500253</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>50</v>
       </c>
@@ -2995,7 +2998,7 @@
         <v>14672.225903446</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
@@ -3039,7 +3042,7 @@
         <v>1442.6348417890099</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
@@ -3083,7 +3086,7 @@
         <v>9213924.9226947706</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
@@ -3127,7 +3130,7 @@
         <v>902.538936330703</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
@@ -3171,7 +3174,7 @@
         <v>131.908222537261</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
@@ -3215,7 +3218,7 @@
         <v>3667.65907859463</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
@@ -3259,7 +3262,7 @@
         <v>376.61924248916699</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>58</v>
       </c>
@@ -3303,7 +3306,7 @@
         <v>215094.035842913</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>59</v>
       </c>
@@ -3347,7 +3350,7 @@
         <v>43062.343594029197</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>60</v>
       </c>
@@ -3391,7 +3394,7 @@
         <v>5468.3561476966397</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>61</v>
       </c>
@@ -3435,7 +3438,7 @@
         <v>897211.64100796904</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>62</v>
       </c>
@@ -3479,7 +3482,7 @@
         <v>282224.36049611203</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>63</v>
       </c>
@@ -3523,7 +3526,7 @@
         <v>438.649703777659</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>64</v>
       </c>
@@ -3567,7 +3570,7 @@
         <v>488.05420463990498</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>65</v>
       </c>
@@ -3611,7 +3614,7 @@
         <v>5565794.4171479698</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>66</v>
       </c>
@@ -3655,7 +3658,7 @@
         <v>4043.8956554889601</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>67</v>
       </c>
@@ -3699,7 +3702,7 @@
         <v>6941.31062887197</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>68</v>
       </c>
@@ -3743,7 +3746,7 @@
         <v>27510.508244735898</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>69</v>
       </c>
@@ -3787,7 +3790,7 @@
         <v>1461.88943051159</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>70</v>
       </c>
@@ -3831,7 +3834,7 @@
         <v>2431.4354575420198</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>71</v>
       </c>
@@ -3875,7 +3878,7 @@
         <v>2377.3790012736499</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>72</v>
       </c>
@@ -3919,7 +3922,7 @@
         <v>1102.1500630057999</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>73</v>
       </c>
@@ -3927,19 +3930,19 @@
         <v>80</v>
       </c>
       <c r="C75">
-        <v>1000</v>
+        <v>23</v>
       </c>
       <c r="D75">
-        <v>4000</v>
+        <v>1139</v>
       </c>
       <c r="E75">
-        <v>128</v>
+        <v>82</v>
       </c>
       <c r="F75">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G75" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H75">
         <v>10</v>
@@ -3963,7 +3966,7 @@
         <v>1163.6031662891501</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>74</v>
       </c>
@@ -3971,19 +3974,19 @@
         <v>81</v>
       </c>
       <c r="C76">
-        <v>23</v>
+        <v>1000</v>
       </c>
       <c r="D76">
-        <v>1139</v>
+        <v>4000</v>
       </c>
       <c r="E76">
-        <v>82</v>
+        <v>128</v>
       </c>
       <c r="F76">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G76" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H76">
         <v>10</v>
@@ -4007,7 +4010,7 @@
         <v>7687.4772859493296</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>75</v>
       </c>
@@ -4051,7 +4054,7 @@
         <v>3405450.27437599</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>76</v>
       </c>
@@ -4095,7 +4098,7 @@
         <v>416883.29775341402</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>77</v>
       </c>
@@ -4139,7 +4142,7 @@
         <v>564039.18658991903</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>78</v>
       </c>
@@ -4183,7 +4186,7 @@
         <v>680532.823463985</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>79</v>
       </c>
@@ -4227,7 +4230,7 @@
         <v>14945.906483103399</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>80</v>
       </c>
@@ -4271,7 +4274,7 @@
         <v>279.33115921885098</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>81</v>
       </c>
@@ -4315,7 +4318,7 @@
         <v>25005.7684203229</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>82</v>
       </c>
@@ -4359,7 +4362,7 @@
         <v>23607.731362460301</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>83</v>
       </c>
@@ -4403,7 +4406,7 @@
         <v>14466.789782336</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>84</v>
       </c>
@@ -4456,13 +4459,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:G1048576"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75:G76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -4503,7 +4506,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -4547,7 +4550,7 @@
         <v>27567.108490749099</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4591,7 +4594,7 @@
         <v>1274.3013183881701</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -4635,7 +4638,7 @@
         <v>1934.04552144422</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -4679,7 +4682,7 @@
         <v>521.84170103271197</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -4723,7 +4726,7 @@
         <v>401.76155374548</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4767,7 +4770,7 @@
         <v>2919.93994013372</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -4811,7 +4814,7 @@
         <v>3008.2664171476999</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -4855,7 +4858,7 @@
         <v>18775.0092634748</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -4899,7 +4902,7 @@
         <v>828414.27276651806</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -4943,7 +4946,7 @@
         <v>326.24289282701397</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -4987,7 +4990,7 @@
         <v>224854.565615795</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -5031,7 +5034,7 @@
         <v>16760.924270936699</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -5075,7 +5078,7 @@
         <v>32830.647783934699</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -5119,7 +5122,7 @@
         <v>20416.555635289002</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -5163,7 +5166,7 @@
         <v>6199.2647767457001</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -5207,7 +5210,7 @@
         <v>244.78077328519899</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -5251,7 +5254,7 @@
         <v>631.60353430597399</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -5295,7 +5298,7 @@
         <v>142.73092235690601</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>21</v>
       </c>
@@ -5339,7 +5342,7 @@
         <v>2738.1336866563302</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
@@ -5383,7 +5386,7 @@
         <v>140.48651194541199</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>19</v>
       </c>
@@ -5427,7 +5430,7 @@
         <v>10192.2010251953</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20</v>
       </c>
@@ -5471,7 +5474,7 @@
         <v>2011.9248563020601</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -5515,7 +5518,7 @@
         <v>146425.17729652199</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -5559,7 +5562,7 @@
         <v>13221.4516852826</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -5603,7 +5606,7 @@
         <v>2333.0641549264401</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -5647,7 +5650,7 @@
         <v>13949.1038287957</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -5691,7 +5694,7 @@
         <v>49880.751921593801</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -5735,7 +5738,7 @@
         <v>9550.8293262357001</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -5779,7 +5782,7 @@
         <v>269784.27518532198</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -5823,7 +5826,7 @@
         <v>336769.01724996098</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -5867,7 +5870,7 @@
         <v>215.59982257120501</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -5911,7 +5914,7 @@
         <v>2200.2041678359601</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -5955,7 +5958,7 @@
         <v>1975954.60750956</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -5999,7 +6002,7 @@
         <v>334550.56713258201</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
@@ -6043,7 +6046,7 @@
         <v>1348.169881327</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -6087,7 +6090,7 @@
         <v>2078021.50824384</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
@@ -6131,7 +6134,7 @@
         <v>45587.5248804742</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -6175,7 +6178,7 @@
         <v>105.164185297166</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
@@ -6219,7 +6222,7 @@
         <v>13344.5920715385</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -6263,7 +6266,7 @@
         <v>2346.2470683952702</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
@@ -6307,7 +6310,7 @@
         <v>1197.31495147136</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
@@ -6351,7 +6354,7 @@
         <v>777654.04896031495</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
@@ -6395,7 +6398,7 @@
         <v>1130.2555836542799</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
@@ -6439,7 +6442,7 @@
         <v>2178.6404165905001</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
@@ -6483,7 +6486,7 @@
         <v>98.708905990789802</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
@@ -6527,7 +6530,7 @@
         <v>391.19813559382197</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
@@ -6571,7 +6574,7 @@
         <v>195.215189152287</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
@@ -6615,7 +6618,7 @@
         <v>929.14773129099603</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
@@ -6659,7 +6662,7 @@
         <v>3830793.38779432</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
@@ -6703,7 +6706,7 @@
         <v>3648723.6935384301</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -6747,7 +6750,7 @@
         <v>873.24672465438596</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>50</v>
       </c>
@@ -6791,7 +6794,7 @@
         <v>9007.4688503493107</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
@@ -6835,7 +6838,7 @@
         <v>629.85496704641503</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
@@ -6879,7 +6882,7 @@
         <v>8940013.5823918004</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
@@ -6923,7 +6926,7 @@
         <v>418.40791213442702</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
@@ -6967,7 +6970,7 @@
         <v>120.000982581538</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
@@ -7011,7 +7014,7 @@
         <v>215.422736122668</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
@@ -7055,7 +7058,7 @@
         <v>297.24191103607001</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>58</v>
       </c>
@@ -7099,7 +7102,7 @@
         <v>27926.8141251983</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>59</v>
       </c>
@@ -7143,7 +7146,7 @@
         <v>14557.329179103501</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>60</v>
       </c>
@@ -7187,7 +7190,7 @@
         <v>6126.4398996898699</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>61</v>
       </c>
@@ -7231,7 +7234,7 @@
         <v>956644.34766829596</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>62</v>
       </c>
@@ -7275,7 +7278,7 @@
         <v>17198.596179928201</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>63</v>
       </c>
@@ -7319,7 +7322,7 @@
         <v>315.85832449655601</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>64</v>
       </c>
@@ -7363,7 +7366,7 @@
         <v>404.12812086361902</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>65</v>
       </c>
@@ -7407,7 +7410,7 @@
         <v>5819553.5210279003</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>66</v>
       </c>
@@ -7451,7 +7454,7 @@
         <v>2694.2920364226402</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>67</v>
       </c>
@@ -7495,7 +7498,7 @@
         <v>4494.5583999562596</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>68</v>
       </c>
@@ -7539,7 +7542,7 @@
         <v>23414.2780545967</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>69</v>
       </c>
@@ -7583,7 +7586,7 @@
         <v>387.41006676539502</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>70</v>
       </c>
@@ -7627,7 +7630,7 @@
         <v>2357.3813058324799</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>71</v>
       </c>
@@ -7671,7 +7674,7 @@
         <v>1837.842896935</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>72</v>
       </c>
@@ -7715,7 +7718,7 @@
         <v>564.50484391691896</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>73</v>
       </c>
@@ -7723,19 +7726,19 @@
         <v>80</v>
       </c>
       <c r="C75">
-        <v>1000</v>
+        <v>23</v>
       </c>
       <c r="D75">
-        <v>4000</v>
+        <v>1139</v>
       </c>
       <c r="E75">
-        <v>128</v>
+        <v>82</v>
       </c>
       <c r="F75">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G75" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H75">
         <v>10</v>
@@ -7759,7 +7762,7 @@
         <v>610.88661228891795</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>74</v>
       </c>
@@ -7767,19 +7770,19 @@
         <v>81</v>
       </c>
       <c r="C76">
-        <v>23</v>
+        <v>1000</v>
       </c>
       <c r="D76">
-        <v>1139</v>
+        <v>4000</v>
       </c>
       <c r="E76">
-        <v>82</v>
+        <v>128</v>
       </c>
       <c r="F76">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G76" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H76">
         <v>10</v>
@@ -7803,7 +7806,7 @@
         <v>9803.4184951261504</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>75</v>
       </c>
@@ -7847,7 +7850,7 @@
         <v>3937780.731782</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>76</v>
       </c>
@@ -7891,7 +7894,7 @@
         <v>80078.019256104293</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>77</v>
       </c>
@@ -7935,7 +7938,7 @@
         <v>72184.730974029604</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>78</v>
       </c>
@@ -7979,7 +7982,7 @@
         <v>40579.356245074501</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>79</v>
       </c>
@@ -8023,7 +8026,7 @@
         <v>9788.9123069106899</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>80</v>
       </c>
@@ -8067,7 +8070,7 @@
         <v>235.02371979906101</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>81</v>
       </c>
@@ -8111,7 +8114,7 @@
         <v>33996.391730734402</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>82</v>
       </c>
@@ -8155,7 +8158,7 @@
         <v>52166.267553887003</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>83</v>
       </c>
@@ -8199,7 +8202,7 @@
         <v>8777.0636082748897</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>84</v>
       </c>
@@ -8252,13 +8255,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75:G76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -8299,7 +8302,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -8343,7 +8346,7 @@
         <v>19820.960782182901</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -8387,7 +8390,7 @@
         <v>2484.9196158270602</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -8431,7 +8434,7 @@
         <v>1677.2555737344401</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -8475,7 +8478,7 @@
         <v>1136.4721355645399</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -8519,7 +8522,7 @@
         <v>955.45419267832403</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -8563,7 +8566,7 @@
         <v>5878.2072368220297</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -8607,7 +8610,7 @@
         <v>4173.1063533038496</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -8651,7 +8654,7 @@
         <v>13460.467844757701</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -8695,7 +8698,7 @@
         <v>3821254.6537963999</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -8739,7 +8742,7 @@
         <v>255.08388787982699</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -8783,7 +8786,7 @@
         <v>24544.911891486601</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -8827,7 +8830,7 @@
         <v>82793.1556077922</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -8871,7 +8874,7 @@
         <v>25361.4234335082</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -8915,7 +8918,7 @@
         <v>13320.5369059525</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -8959,7 +8962,7 @@
         <v>5324.8396835383901</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -9003,7 +9006,7 @@
         <v>194.29365132221901</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -9047,7 +9050,7 @@
         <v>439.638312706139</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -9091,7 +9094,7 @@
         <v>228.16853149062101</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>21</v>
       </c>
@@ -9135,7 +9138,7 @@
         <v>9733.2845048929903</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
@@ -9179,7 +9182,7 @@
         <v>209.873350630472</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>19</v>
       </c>
@@ -9223,7 +9226,7 @@
         <v>14556.650227537701</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20</v>
       </c>
@@ -9267,7 +9270,7 @@
         <v>2886.2479117856801</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -9311,7 +9314,7 @@
         <v>243716.17611032599</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -9355,7 +9358,7 @@
         <v>30977.324064926601</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -9399,7 +9402,7 @@
         <v>2932.33188571865</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -9443,7 +9446,7 @@
         <v>20971.698606775</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -9487,7 +9490,7 @@
         <v>44858.952695471198</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -9531,7 +9534,7 @@
         <v>7364.5541565457597</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -9575,7 +9578,7 @@
         <v>1044854.02684697</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -9619,7 +9622,7 @@
         <v>518311.37132663402</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -9663,7 +9666,7 @@
         <v>337.51159446150899</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -9707,7 +9710,7 @@
         <v>5281.3739375083796</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -9751,7 +9754,7 @@
         <v>4739023.5022926396</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -9795,7 +9798,7 @@
         <v>71174.532640953097</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
@@ -9839,7 +9842,7 @@
         <v>2052.1157384670801</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -9883,7 +9886,7 @@
         <v>3700720.3498964701</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
@@ -9927,7 +9930,7 @@
         <v>68012.849193212896</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -9971,7 +9974,7 @@
         <v>120.615774605807</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
@@ -10015,7 +10018,7 @@
         <v>34661.393747579197</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -10059,7 +10062,7 @@
         <v>4184.9407526732302</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
@@ -10103,7 +10106,7 @@
         <v>4292.5017137874302</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
@@ -10147,7 +10150,7 @@
         <v>2870088.4775855402</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
@@ -10191,7 +10194,7 @@
         <v>1892.1188835513301</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
@@ -10235,7 +10238,7 @@
         <v>4412.1646110948996</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
@@ -10279,7 +10282,7 @@
         <v>173.92567361889101</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
@@ -10323,7 +10326,7 @@
         <v>518.10097768070602</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
@@ -10367,7 +10370,7 @@
         <v>1021.00406985572</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
@@ -10411,7 +10414,7 @@
         <v>1475.37652766719</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
@@ -10455,7 +10458,7 @@
         <v>3261750.3265373199</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
@@ -10499,7 +10502,7 @@
         <v>4996783.3243305404</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -10543,7 +10546,7 @@
         <v>2222.5073594577202</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>50</v>
       </c>
@@ -10587,7 +10590,7 @@
         <v>7051.1236531217701</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
@@ -10631,7 +10634,7 @@
         <v>1244.1810701731399</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
@@ -10675,7 +10678,7 @@
         <v>8559790.2343925405</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
@@ -10719,7 +10722,7 @@
         <v>746.05388451794204</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
@@ -10763,7 +10766,7 @@
         <v>307.51868531919899</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
@@ -10807,7 +10810,7 @@
         <v>619.175666380385</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
@@ -10851,7 +10854,7 @@
         <v>328.15744545941197</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>58</v>
       </c>
@@ -10895,7 +10898,7 @@
         <v>45135.378825562198</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>59</v>
       </c>
@@ -10939,7 +10942,7 @@
         <v>21228.076937485101</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>60</v>
       </c>
@@ -10983,7 +10986,7 @@
         <v>14404.0359544896</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>61</v>
       </c>
@@ -11027,7 +11030,7 @@
         <v>237346.082632192</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>62</v>
       </c>
@@ -11071,7 +11074,7 @@
         <v>25002.848302887</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>63</v>
       </c>
@@ -11115,7 +11118,7 @@
         <v>680.93145685570005</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>64</v>
       </c>
@@ -11159,7 +11162,7 @@
         <v>686.88140528652002</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>65</v>
       </c>
@@ -11203,7 +11206,7 @@
         <v>7997868.9239492798</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>66</v>
       </c>
@@ -11247,7 +11250,7 @@
         <v>6308.5939624290004</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>67</v>
       </c>
@@ -11291,7 +11294,7 @@
         <v>6632.5451539866699</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>68</v>
       </c>
@@ -11335,7 +11338,7 @@
         <v>38923.103631399201</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>69</v>
       </c>
@@ -11379,7 +11382,7 @@
         <v>454.54665970891898</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>70</v>
       </c>
@@ -11423,7 +11426,7 @@
         <v>2806.4784311753301</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>71</v>
       </c>
@@ -11467,7 +11470,7 @@
         <v>3109.72454833441</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>72</v>
       </c>
@@ -11511,7 +11514,7 @@
         <v>4123.4227712858201</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>73</v>
       </c>
@@ -11519,19 +11522,19 @@
         <v>80</v>
       </c>
       <c r="C75">
-        <v>1000</v>
+        <v>23</v>
       </c>
       <c r="D75">
-        <v>4000</v>
+        <v>1139</v>
       </c>
       <c r="E75">
-        <v>128</v>
+        <v>82</v>
       </c>
       <c r="F75">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G75" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H75">
         <v>10</v>
@@ -11555,7 +11558,7 @@
         <v>1382.66141685562</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>74</v>
       </c>
@@ -11563,19 +11566,19 @@
         <v>81</v>
       </c>
       <c r="C76">
-        <v>23</v>
+        <v>1000</v>
       </c>
       <c r="D76">
-        <v>1139</v>
+        <v>4000</v>
       </c>
       <c r="E76">
-        <v>82</v>
+        <v>128</v>
       </c>
       <c r="F76">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G76" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H76">
         <v>10</v>
@@ -11599,7 +11602,7 @@
         <v>102309.781877149</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>75</v>
       </c>
@@ -11643,7 +11646,7 @@
         <v>2243998.3240612801</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>76</v>
       </c>
@@ -11687,7 +11690,7 @@
         <v>630391.651508832</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>77</v>
       </c>
@@ -11731,7 +11734,7 @@
         <v>736334.58814204601</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>78</v>
       </c>
@@ -11775,7 +11778,7 @@
         <v>99422.854471668004</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>79</v>
       </c>
@@ -11819,7 +11822,7 @@
         <v>18002.822832418798</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>80</v>
       </c>
@@ -11863,7 +11866,7 @@
         <v>346.92137220369398</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>81</v>
       </c>
@@ -11907,7 +11910,7 @@
         <v>63490.5686307285</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>82</v>
       </c>
@@ -11951,7 +11954,7 @@
         <v>12397.576563762899</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>83</v>
       </c>
@@ -11995,7 +11998,7 @@
         <v>105974.912169123</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>84</v>
       </c>

</xml_diff>